<commit_message>
added the ability to edit the left table on leftclick
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>Category</t>
   </si>
@@ -102,6 +102,30 @@
   </si>
   <si>
     <t>444444.0</t>
+  </si>
+  <si>
+    <t>1202.0</t>
+  </si>
+  <si>
+    <t>1200.0</t>
+  </si>
+  <si>
+    <t>smwms</t>
+  </si>
+  <si>
+    <t>2023-03-14</t>
+  </si>
+  <si>
+    <t>smwm</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>swsd</t>
+  </si>
+  <si>
+    <t>450.0</t>
   </si>
 </sst>
 </file>
@@ -152,7 +176,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -328,6 +352,91 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
excel now creates a sheet that corresponds to the month of the expense
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -6,13 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="mars" r:id="rId3" sheetId="1"/>
+    <sheet name="april" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
   <si>
     <t>Category</t>
   </si>
@@ -126,6 +127,33 @@
   </si>
   <si>
     <t>450.0</t>
+  </si>
+  <si>
+    <t>sws</t>
+  </si>
+  <si>
+    <t>2023-03-15</t>
+  </si>
+  <si>
+    <t>123.0</t>
+  </si>
+  <si>
+    <t>343.0</t>
+  </si>
+  <si>
+    <t>2024-03-13</t>
+  </si>
+  <si>
+    <t>5454.0</t>
+  </si>
+  <si>
+    <t>dfsf</t>
+  </si>
+  <si>
+    <t>2023-04-12</t>
+  </si>
+  <si>
+    <t>342.0</t>
   </si>
 </sst>
 </file>
@@ -133,18 +161,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,35 +190,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -434,6 +456,104 @@
         <v>37</v>
       </c>
       <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed the menu, so that each window is unique
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
-    <sheet name="april" r:id="rId4" sheetId="2"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>

<commit_message>
Created method and class to create user, and added hash to passwords
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Category</t>
   </si>
@@ -83,7 +84,7 @@
     <t>Transportation</t>
   </si>
   <si>
-    <t>AtB månedskort</t>
+    <t>AtB mÃ¥nedskort</t>
   </si>
   <si>
     <t>2023-03-13</t>
@@ -92,22 +93,31 @@
     <t>550.0</t>
   </si>
   <si>
-    <t>onlyfans</t>
+    <t>asdfg</t>
   </si>
   <si>
     <t>2023-03-15</t>
   </si>
   <si>
+    <t>1000.0</t>
+  </si>
+  <si>
+    <t>HYRE</t>
+  </si>
+  <si>
+    <t>2023-03-16</t>
+  </si>
+  <si>
+    <t>150.0</t>
+  </si>
+  <si>
+    <t>gucci sokker</t>
+  </si>
+  <si>
+    <t>2023-04-06</t>
+  </si>
+  <si>
     <t>2000.0</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>asdfg</t>
-  </si>
-  <si>
-    <t>1000.0</t>
   </si>
 </sst>
 </file>
@@ -262,7 +272,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -274,24 +284,71 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added enter fucntionality so you dont have to press the buttons
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Category</t>
   </si>
@@ -84,7 +84,7 @@
     <t>Transportation</t>
   </si>
   <si>
-    <t>AtB mÃ¥nedskort</t>
+    <t>AtB månedskort</t>
   </si>
   <si>
     <t>2023-03-13</t>
@@ -93,31 +93,46 @@
     <t>550.0</t>
   </si>
   <si>
-    <t>asdfg</t>
-  </si>
-  <si>
-    <t>2023-03-15</t>
+    <t>HYRE</t>
+  </si>
+  <si>
+    <t>2023-03-16</t>
+  </si>
+  <si>
+    <t>150.0</t>
+  </si>
+  <si>
+    <t>gucci sokker</t>
+  </si>
+  <si>
+    <t>2023-04-06</t>
+  </si>
+  <si>
+    <t>2000.0</t>
+  </si>
+  <si>
+    <t>pizza</t>
+  </si>
+  <si>
+    <t>2023-03-09</t>
   </si>
   <si>
     <t>1000.0</t>
   </si>
   <si>
-    <t>HYRE</t>
-  </si>
-  <si>
-    <t>2023-03-16</t>
-  </si>
-  <si>
-    <t>150.0</t>
-  </si>
-  <si>
-    <t>gucci sokker</t>
-  </si>
-  <si>
-    <t>2023-04-06</t>
-  </si>
-  <si>
-    <t>2000.0</t>
+    <t>buss</t>
+  </si>
+  <si>
+    <t>2023-03-18</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>sdaf</t>
+  </si>
+  <si>
+    <t>1234.0</t>
   </si>
 </sst>
 </file>
@@ -162,7 +177,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -272,7 +287,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -284,24 +299,58 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
-        <v>14</v>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -339,13 +388,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
created duplicate in right table, added test test user
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -6,14 +6,15 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="March" r:id="rId3" sheetId="1"/>
-    <sheet name="April" r:id="rId4" sheetId="2"/>
+    <sheet name="mars" r:id="rId3" sheetId="1"/>
+    <sheet name="april" r:id="rId4" sheetId="2"/>
+    <sheet name="mai" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>Category</t>
   </si>
@@ -84,7 +85,7 @@
     <t>Transportation</t>
   </si>
   <si>
-    <t>AtB månedskort</t>
+    <t>AtB mÃ¥nedskort</t>
   </si>
   <si>
     <t>2023-03-13</t>
@@ -133,6 +134,21 @@
   </si>
   <si>
     <t>1234.0</t>
+  </si>
+  <si>
+    <t>flybillett</t>
+  </si>
+  <si>
+    <t>2023-05-23</t>
+  </si>
+  <si>
+    <t>450.0</t>
+  </si>
+  <si>
+    <t>frf</t>
+  </si>
+  <si>
+    <t>434.0</t>
   </si>
 </sst>
 </file>
@@ -403,4 +419,68 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>